<commit_message>
video files added 20180117
video files added 20180117
</commit_message>
<xml_diff>
--- a/Develop/영상처리.xlsx
+++ b/Develop/영상처리.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="495">
   <si>
     <t>기하와벡터</t>
   </si>
@@ -1553,6 +1553,15 @@
   </si>
   <si>
     <t>62b0e17cb06928eec8d1bc1f8317f6fd1a88560869ed090c801c34e81c8727b4</t>
+  </si>
+  <si>
+    <t>eba10ae0e9b760bf86eaba260f6eb8df2373bd2efd275a4974b8b182387f86ff</t>
+  </si>
+  <si>
+    <t>9b3fa5098bfe8766cb79fb5d4809a8aa89f5b2cec60f27c767d718f1e4c061d3</t>
+  </si>
+  <si>
+    <t>e32400b64fabd03c90d9b0ec322c95b6f89ae0023454fd5c23b0ae22ec9a0c14</t>
   </si>
 </sst>
 </file>
@@ -1931,11 +1940,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J467"/>
+  <dimension ref="A1:J470"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A451" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A468" sqref="A468"/>
+      <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J470" sqref="J470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -17058,6 +17067,84 @@
       </c>
       <c r="J467" t="s">
         <v>491</v>
+      </c>
+    </row>
+    <row r="468" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A468">
+        <v>467</v>
+      </c>
+      <c r="B468" t="s">
+        <v>64</v>
+      </c>
+      <c r="C468">
+        <v>4</v>
+      </c>
+      <c r="D468" t="s">
+        <v>424</v>
+      </c>
+      <c r="F468">
+        <v>4</v>
+      </c>
+      <c r="H468">
+        <v>95</v>
+      </c>
+      <c r="I468">
+        <v>431</v>
+      </c>
+      <c r="J468" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="469" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A469">
+        <v>468</v>
+      </c>
+      <c r="B469" t="s">
+        <v>64</v>
+      </c>
+      <c r="C469">
+        <v>4</v>
+      </c>
+      <c r="D469" t="s">
+        <v>424</v>
+      </c>
+      <c r="F469">
+        <v>4</v>
+      </c>
+      <c r="H469">
+        <v>101</v>
+      </c>
+      <c r="I469">
+        <v>432</v>
+      </c>
+      <c r="J469" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="470" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A470">
+        <v>469</v>
+      </c>
+      <c r="B470" t="s">
+        <v>64</v>
+      </c>
+      <c r="C470">
+        <v>4</v>
+      </c>
+      <c r="D470" t="s">
+        <v>424</v>
+      </c>
+      <c r="F470">
+        <v>4</v>
+      </c>
+      <c r="H470">
+        <v>168</v>
+      </c>
+      <c r="I470">
+        <v>433</v>
+      </c>
+      <c r="J470" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
submitmyQuestion 함수 변경 제안
submitmyQuestion 함수 변경 제안
</commit_message>
<xml_diff>
--- a/Develop/영상처리.xlsx
+++ b/Develop/영상처리.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="500">
   <si>
     <t>기하와벡터</t>
   </si>
@@ -1562,6 +1562,21 @@
   </si>
   <si>
     <t>e32400b64fabd03c90d9b0ec322c95b6f89ae0023454fd5c23b0ae22ec9a0c14</t>
+  </si>
+  <si>
+    <t>f31c982609189dbd1db2c2528d115b8ba128a592ed8bab31fbf4350c3662b1e0</t>
+  </si>
+  <si>
+    <t>195cb072d8111911c917d23f7e550e9adcea4cfbc472af2b889a95019b3cc4ab</t>
+  </si>
+  <si>
+    <t>6187f3b478d29339808d72e692960dcdf64aabffdd01a944f46a22dc33575db4</t>
+  </si>
+  <si>
+    <t>e953bf0f136112b1e149473de05bae0e0921a9dd998e7a701bb36a3c3206a798</t>
+  </si>
+  <si>
+    <t>54faea9b3eeffce2a5ea906fdd1232a52a55d57d993e5406a572b9a9ea2827d8</t>
   </si>
 </sst>
 </file>
@@ -1940,11 +1955,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J470"/>
+  <dimension ref="A1:J475"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A455" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J470" sqref="J470"/>
+      <pane ySplit="1" topLeftCell="A457" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A476" sqref="A476"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -17145,6 +17160,136 @@
       </c>
       <c r="J470" t="s">
         <v>494</v>
+      </c>
+    </row>
+    <row r="471" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A471">
+        <v>470</v>
+      </c>
+      <c r="B471" t="s">
+        <v>64</v>
+      </c>
+      <c r="C471">
+        <v>4</v>
+      </c>
+      <c r="D471" t="s">
+        <v>424</v>
+      </c>
+      <c r="F471">
+        <v>4</v>
+      </c>
+      <c r="H471">
+        <v>178</v>
+      </c>
+      <c r="I471">
+        <v>436</v>
+      </c>
+      <c r="J471" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="472" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A472">
+        <v>471</v>
+      </c>
+      <c r="B472" t="s">
+        <v>64</v>
+      </c>
+      <c r="C472">
+        <v>4</v>
+      </c>
+      <c r="D472" t="s">
+        <v>424</v>
+      </c>
+      <c r="F472">
+        <v>4</v>
+      </c>
+      <c r="H472">
+        <v>180</v>
+      </c>
+      <c r="I472">
+        <v>437</v>
+      </c>
+      <c r="J472" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="473" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A473">
+        <v>472</v>
+      </c>
+      <c r="B473" t="s">
+        <v>64</v>
+      </c>
+      <c r="C473">
+        <v>4</v>
+      </c>
+      <c r="D473" t="s">
+        <v>424</v>
+      </c>
+      <c r="F473">
+        <v>4</v>
+      </c>
+      <c r="H473">
+        <v>196</v>
+      </c>
+      <c r="I473">
+        <v>438</v>
+      </c>
+      <c r="J473" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="474" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A474">
+        <v>473</v>
+      </c>
+      <c r="B474" t="s">
+        <v>64</v>
+      </c>
+      <c r="C474">
+        <v>4</v>
+      </c>
+      <c r="D474" t="s">
+        <v>424</v>
+      </c>
+      <c r="F474">
+        <v>4</v>
+      </c>
+      <c r="H474">
+        <v>197</v>
+      </c>
+      <c r="I474">
+        <v>439</v>
+      </c>
+      <c r="J474" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="475" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A475">
+        <v>474</v>
+      </c>
+      <c r="B475" t="s">
+        <v>64</v>
+      </c>
+      <c r="C475">
+        <v>4</v>
+      </c>
+      <c r="D475" t="s">
+        <v>424</v>
+      </c>
+      <c r="F475">
+        <v>4</v>
+      </c>
+      <c r="H475">
+        <v>199</v>
+      </c>
+      <c r="I475">
+        <v>440</v>
+      </c>
+      <c r="J475" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>